<commit_message>
poprawki na mobilne + pusta baza danych
</commit_message>
<xml_diff>
--- a/Pluton.xlsx
+++ b/Pluton.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/maciek/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/maciek/PycharmProjects/AppDjango/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5FBDEE12-697E-ED49-A6D4-497FDD475B3F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52D1F8CC-AAF1-6242-9C60-6D1D8128970A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="39600" yWindow="1700" windowWidth="28240" windowHeight="17560" xr2:uid="{A5AC1BB9-6F6C-534B-A730-39A313905F29}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="20080" xr2:uid="{A5AC1BB9-6F6C-534B-A730-39A313905F29}"/>
   </bookViews>
   <sheets>
     <sheet name="Arkusz1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="56">
   <si>
     <t>Paweł</t>
   </si>
@@ -198,6 +198,9 @@
   </si>
   <si>
     <t>Krzysztof</t>
+  </si>
+  <si>
+    <t>pchor.</t>
   </si>
 </sst>
 </file>
@@ -574,7 +577,7 @@
   <dimension ref="A1:E35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G28" sqref="G28"/>
+      <selection sqref="A1:A35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -583,8 +586,8 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1">
-        <v>1</v>
+      <c r="A1" t="s">
+        <v>55</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -600,8 +603,8 @@
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2">
-        <v>2</v>
+      <c r="A2" t="s">
+        <v>55</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>1</v>
@@ -617,8 +620,8 @@
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3">
-        <v>3</v>
+      <c r="A3" t="s">
+        <v>55</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>0</v>
@@ -634,8 +637,8 @@
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4">
-        <v>4</v>
+      <c r="A4" t="s">
+        <v>55</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>2</v>
@@ -651,8 +654,8 @@
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5">
-        <v>5</v>
+      <c r="A5" t="s">
+        <v>55</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>3</v>
@@ -668,8 +671,8 @@
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A6">
-        <v>6</v>
+      <c r="A6" t="s">
+        <v>55</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>4</v>
@@ -685,8 +688,8 @@
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A7">
-        <v>7</v>
+      <c r="A7" t="s">
+        <v>55</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>5</v>
@@ -702,8 +705,8 @@
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A8">
-        <v>8</v>
+      <c r="A8" t="s">
+        <v>55</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>6</v>
@@ -719,8 +722,8 @@
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A9">
-        <v>9</v>
+      <c r="A9" t="s">
+        <v>55</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>7</v>
@@ -736,8 +739,8 @@
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A10">
-        <v>10</v>
+      <c r="A10" t="s">
+        <v>55</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>8</v>
@@ -753,8 +756,8 @@
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A11">
-        <v>11</v>
+      <c r="A11" t="s">
+        <v>55</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>0</v>
@@ -770,8 +773,8 @@
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A12">
-        <v>12</v>
+      <c r="A12" t="s">
+        <v>55</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>1</v>
@@ -787,8 +790,8 @@
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A13">
-        <v>13</v>
+      <c r="A13" t="s">
+        <v>55</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>9</v>
@@ -804,8 +807,8 @@
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A14">
-        <v>14</v>
+      <c r="A14" t="s">
+        <v>55</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>10</v>
@@ -821,8 +824,8 @@
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A15">
-        <v>15</v>
+      <c r="A15" t="s">
+        <v>55</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>9</v>
@@ -838,8 +841,8 @@
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A16">
-        <v>16</v>
+      <c r="A16" t="s">
+        <v>55</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>11</v>
@@ -855,8 +858,8 @@
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A17">
-        <v>17</v>
+      <c r="A17" t="s">
+        <v>55</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>12</v>
@@ -872,8 +875,8 @@
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A18">
-        <v>18</v>
+      <c r="A18" t="s">
+        <v>55</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>30</v>
@@ -889,8 +892,8 @@
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A19">
-        <v>19</v>
+      <c r="A19" t="s">
+        <v>55</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>31</v>
@@ -906,8 +909,8 @@
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A20">
-        <v>20</v>
+      <c r="A20" t="s">
+        <v>55</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>9</v>
@@ -923,8 +926,8 @@
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A21">
-        <v>21</v>
+      <c r="A21" t="s">
+        <v>55</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>1</v>
@@ -940,8 +943,8 @@
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A22">
-        <v>22</v>
+      <c r="A22" t="s">
+        <v>55</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>6</v>
@@ -957,8 +960,8 @@
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A23">
-        <v>23</v>
+      <c r="A23" t="s">
+        <v>55</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>32</v>
@@ -974,8 +977,8 @@
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A24">
-        <v>24</v>
+      <c r="A24" t="s">
+        <v>55</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>33</v>
@@ -991,8 +994,8 @@
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A25">
-        <v>25</v>
+      <c r="A25" t="s">
+        <v>55</v>
       </c>
       <c r="B25" s="1" t="s">
         <v>32</v>
@@ -1008,8 +1011,8 @@
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A26">
-        <v>26</v>
+      <c r="A26" t="s">
+        <v>55</v>
       </c>
       <c r="B26" s="1" t="s">
         <v>32</v>
@@ -1025,8 +1028,8 @@
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A27">
-        <v>27</v>
+      <c r="A27" t="s">
+        <v>55</v>
       </c>
       <c r="B27" s="1" t="s">
         <v>31</v>
@@ -1042,8 +1045,8 @@
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A28">
-        <v>28</v>
+      <c r="A28" t="s">
+        <v>55</v>
       </c>
       <c r="B28" s="1" t="s">
         <v>1</v>
@@ -1059,8 +1062,8 @@
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A29">
-        <v>29</v>
+      <c r="A29" t="s">
+        <v>55</v>
       </c>
       <c r="B29" s="1" t="s">
         <v>33</v>
@@ -1076,8 +1079,8 @@
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A30">
-        <v>30</v>
+      <c r="A30" t="s">
+        <v>55</v>
       </c>
       <c r="B30" s="1" t="s">
         <v>33</v>
@@ -1093,8 +1096,8 @@
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A31">
-        <v>31</v>
+      <c r="A31" t="s">
+        <v>55</v>
       </c>
       <c r="B31" s="1" t="s">
         <v>54</v>
@@ -1110,8 +1113,8 @@
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A32">
-        <v>32</v>
+      <c r="A32" t="s">
+        <v>55</v>
       </c>
       <c r="B32" s="1" t="s">
         <v>32</v>
@@ -1127,8 +1130,8 @@
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A33">
-        <v>33</v>
+      <c r="A33" t="s">
+        <v>55</v>
       </c>
       <c r="B33" s="1" t="s">
         <v>34</v>
@@ -1144,8 +1147,8 @@
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A34">
-        <v>34</v>
+      <c r="A34" t="s">
+        <v>55</v>
       </c>
       <c r="B34" s="1" t="s">
         <v>35</v>
@@ -1161,8 +1164,8 @@
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A35">
-        <v>35</v>
+      <c r="A35" t="s">
+        <v>55</v>
       </c>
       <c r="B35" s="1" t="s">
         <v>1</v>

</xml_diff>